<commit_message>
user study section polishing
</commit_message>
<xml_diff>
--- a/Chameleon/Figures/questionnaires.xlsx
+++ b/Chameleon/Figures/questionnaires.xlsx
@@ -14,6 +14,10 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$28:$B$32</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$28:$B$32</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,9 +28,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Compartment</t>
+  </si>
+  <si>
+    <t>Capsid proteins</t>
+  </si>
+  <si>
+    <t>Protein domain</t>
+  </si>
+  <si>
+    <t>secondary str.</t>
   </si>
   <si>
     <t>Atomic structure</t>
@@ -39,6 +52,24 @@
   </si>
   <si>
     <t>Secondary structures</t>
+  </si>
+  <si>
+    <t>notice</t>
+  </si>
+  <si>
+    <t>confused</t>
+  </si>
+  <si>
+    <t>understood strategy</t>
+  </si>
+  <si>
+    <t>Notice color change</t>
+  </si>
+  <si>
+    <t>Confusion by color change</t>
+  </si>
+  <si>
+    <t>Visual appeal</t>
   </si>
 </sst>
 </file>
@@ -68,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -91,11 +122,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -103,9 +145,16 @@
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,6 +206,72 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$B$20:$F$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.19999999999999996</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.44721359549995793</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.48989794855663565</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.54772255750516607</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.40000000000000019</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$B$20:$F$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.19999999999999996</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.44721359549995793</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.48989794855663565</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.54772255750516607</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.40000000000000019</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$2:$F$2</c:f>
@@ -272,6 +387,7 @@
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
@@ -373,7 +489,898 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$B$36:$D$36</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.77459666924148329</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.44721359549995793</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.50990195135927863</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$B$36:$D$36</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.77459666924148329</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.44721359549995793</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.50990195135927863</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$27:$D$27</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>notice</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>confused</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>understood strategy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$34:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8F15-4FBB-AA57-7C405B6BAAD7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="2020954256"/>
+        <c:axId val="2020956752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2020954256"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2020956752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2020956752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2020954256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.32322134733158353"/>
+          <c:y val="0.15832531350247886"/>
+          <c:w val="0.65377865266841639"/>
+          <c:h val="0.8416746864975212"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-CF02-49AC-AA55-AC9876FEB2C2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-CF02-49AC-AA55-AC9876FEB2C2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-CF02-49AC-AA55-AC9876FEB2C2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-CF02-49AC-AA55-AC9876FEB2C2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-CF02-49AC-AA55-AC9876FEB2C2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-CF02-49AC-AA55-AC9876FEB2C2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-CF02-49AC-AA55-AC9876FEB2C2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-CF02-49AC-AA55-AC9876FEB2C2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$B$20:$I$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>0.19999999999999996</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.44721359549995793</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.48989794855663565</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.54772255750516607</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.40000000000000019</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.77459666924148329</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.44721359549995793</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$B$20:$I$20</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>0.19999999999999996</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.44721359549995793</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.48989794855663565</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.54772255750516607</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.40000000000000019</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.77459666924148329</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.44721359549995793</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Compartment</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Capsid protein</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Protein domains</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Secondary structures</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Atomic structure</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Notice color change</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Confusion by color change</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Visual appeal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CF02-49AC-AA55-AC9876FEB2C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="65"/>
+        <c:axId val="94133728"/>
+        <c:axId val="94142048"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="94133728"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="94142048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="94142048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="95000"/>
+                      <a:lumOff val="5000"/>
+                      <a:alpha val="42000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="36000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="94133728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -418,6 +1425,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -923,20 +2010,1095 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="218">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>49800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -950,6 +3112,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>138112</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>442912</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>261937</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1221,49 +3443,359 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:6" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="4">
+        <v>4.8</v>
+      </c>
+      <c r="C3" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F3" s="4">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="I3" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3">
+        <v>5</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3">
+        <v>4</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>5</v>
+      </c>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3">
+        <v>5</v>
+      </c>
+      <c r="F16" s="3">
+        <v>5</v>
+      </c>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>AVERAGE(B12:B16)</f>
         <v>4.8</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C18">
+        <f t="shared" ref="C18:J19" si="0">AVERAGE(C12:C16)</f>
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="D3" s="3">
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f>_xlfn.STDEV.S(B12:B16)</f>
+        <v>0.44721359549995787</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:J19" si="1">_xlfn.STDEV.S(C12:C16)</f>
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>1.0954451150103324</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>1.2247448713915889</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0.8944271909999163</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f>B19/SQRT(5)</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:F20" si="2">C19/SQRT(5)</f>
+        <v>0.44721359549995793</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>0.48989794855663565</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>0.54772255750516607</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>0.40000000000000019</v>
+      </c>
+      <c r="G20">
+        <v>0.77459666924148329</v>
+      </c>
+      <c r="H20">
+        <v>0.44721359549995793</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:9" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="3">
+        <v>5</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
         <v>3</v>
       </c>
-      <c r="E3" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F3" s="3">
+    </row>
+    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="3">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3">
         <v>3</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="3">
+        <v>4</v>
+      </c>
+      <c r="C31" s="3">
+        <v>3</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="3">
+        <v>5</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
+      <c r="D32" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <f>AVERAGE(B28:B32)</f>
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:D34" si="3">AVERAGE(C28:C32)</f>
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="3"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f>_xlfn.STDEV.S(B28:B32)</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:D35" si="4">_xlfn.STDEV.S(C28:C32)</f>
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="4"/>
+        <v>1.1401754250991383</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <f>B35/SQRT(5)</f>
+        <v>0.77459666924148329</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:D36" si="5">C35/SQRT(5)</f>
+        <v>0.44721359549995793</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="5"/>
+        <v>0.50990195135927863</v>
       </c>
     </row>
   </sheetData>

</xml_diff>